<commit_message>
add older catch limits.
</commit_message>
<xml_diff>
--- a/data/data_raw/catchHistory/Landings_FY1997.xlsx
+++ b/data/data_raw/catchHistory/Landings_FY1997.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\min-yang.lee\Downloads\catches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Groundfish-MSE\data\data_raw\catchHistory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -139,17 +139,6 @@
         <family val="2"/>
       </rPr>
       <t>Pollock</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Redfish - 500s</t>
     </r>
   </si>
   <si>
@@ -439,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -479,6 +468,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,7 +779,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -804,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -813,13 +805,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -833,7 +825,7 @@
         <v>1997</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -851,10 +843,10 @@
         <v>1997</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -872,10 +864,10 @@
         <v>1997</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -889,7 +881,7 @@
         <v>1997</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -905,10 +897,10 @@
         <v>1997</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -926,10 +918,10 @@
         <v>1997</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -943,7 +935,7 @@
         <v>1997</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -959,10 +951,10 @@
         <v>1997</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -980,10 +972,10 @@
         <v>1997</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1001,10 +993,10 @@
         <v>1997</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -1016,24 +1008,29 @@
         <v>1997</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>11462</v>
+      </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <f>B13/0.2</f>
+        <v>57310</v>
+      </c>
       <c r="E13">
         <v>1997</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1045,24 +1042,28 @@
         <v>1997</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3"/>
+      <c r="A15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3">
+        <v>526</v>
+      </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>52600</v>
+      </c>
       <c r="E15">
         <v>1997</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1074,26 +1075,29 @@
         <v>1997</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2">
         <v>4937</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <f>B17/0.09</f>
+        <v>54855.555555555555</v>
+      </c>
       <c r="E17">
         <v>1997</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1105,31 +1109,34 @@
         <v>1997</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2">
         <v>8502</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
+      <c r="D19" s="2">
+        <f>B19/0.15</f>
+        <v>56680</v>
+      </c>
       <c r="E19">
         <v>1997</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -1138,7 +1145,7 @@
         <v>1997</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1154,10 +1161,10 @@
         <v>1997</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1173,10 +1180,10 @@
         <v>1997</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1192,10 +1199,10 @@
         <v>1997</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -1207,31 +1214,34 @@
         <v>1997</v>
       </c>
       <c r="G24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2">
         <v>4144</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <f>B25/0.07</f>
+        <v>59199.999999999993</v>
+      </c>
       <c r="E25">
         <v>1997</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -1240,12 +1250,12 @@
         <v>1997</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="3">
         <v>1171</v>
@@ -1256,15 +1266,15 @@
         <v>1997</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="3">
         <v>207</v>
@@ -1275,10 +1285,10 @@
         <v>1997</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -1290,12 +1300,12 @@
         <v>1997</v>
       </c>
       <c r="G29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="1"/>
@@ -1304,15 +1314,15 @@
         <v>1997</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
@@ -1321,12 +1331,12 @@
         <v>1997</v>
       </c>
       <c r="G31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
@@ -1335,12 +1345,12 @@
         <v>1997</v>
       </c>
       <c r="G32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
@@ -1349,7 +1359,7 @@
         <v>1997</v>
       </c>
       <c r="G33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>